<commit_message>
[BI-1613] - More unit test updates
</commit_message>
<xml_diff>
--- a/src/test/resources/files/missing_scale_class.xlsx
+++ b/src/test/resources/files/missing_scale_class.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daw279\Documents\Releases\v0.5\Issues\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hms243/IdeaProjects/bi-api/src/test/resources/files/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C19D1AE5-C415-DB4F-BB1D-C0E68F9F100B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7056"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="31020" windowHeight="14560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Template" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
   <si>
     <t>ALFALFA SNOUT BEETLE</t>
   </si>
@@ -159,12 +160,21 @@
   </si>
   <si>
     <t>alfSnotBeetl</t>
+  </si>
+  <si>
+    <t>Term Type</t>
+  </si>
+  <si>
+    <t>germplasm passport</t>
+  </si>
+  <si>
+    <t>PHENOTYPE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -264,9 +274,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -276,6 +285,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -556,224 +567,236 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:R6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.05078125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7890625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.62890625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.15625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="4.62890625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.41796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.3125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="42.05078125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5234375" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.47265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.05078125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.26171875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="18.83984375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.05078125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="42" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="16" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="6" customFormat="1" ht="15.6" x14ac:dyDescent="0.6">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:18" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="4" t="s">
+      <c r="J1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="K1" s="4" t="s">
+      <c r="L1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="M1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="P1" s="4" t="s">
+      <c r="Q1" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q1" s="5" t="s">
+      <c r="R1" s="4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="7" t="s">
+      <c r="C2" s="8"/>
+      <c r="D2" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7" t="s">
+      <c r="H2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="7" t="s">
+      <c r="I2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" s="7" t="s">
+      <c r="K2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="7" t="s">
+      <c r="M2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M2" s="8"/>
-      <c r="Q2" s="8"/>
+      <c r="N2" s="7"/>
+      <c r="R2" s="7"/>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="8"/>
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="7" t="s">
+      <c r="H3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="7" t="s">
+      <c r="I3" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>34</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="K3" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="M3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M3" s="8"/>
-      <c r="Q3" s="8"/>
+      <c r="N3" s="7"/>
+      <c r="R3" s="7"/>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="6" t="s">
         <v>32</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="H4" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="7" t="s">
+      <c r="I4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="7" t="s">
+      <c r="K4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L4" s="7"/>
-      <c r="M4" s="8"/>
-      <c r="Q4" s="8"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="7"/>
+      <c r="R4" s="7"/>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A5" s="7" t="s">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
         <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7" t="s">
+      <c r="C5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="H5" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="7" t="s">
+      <c r="I5" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="K5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="M5" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M5" s="8"/>
-      <c r="Q5" s="8"/>
+      <c r="N5" s="7"/>
+      <c r="R5" s="7"/>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
         <v>38</v>
       </c>
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="H6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H6" s="7" t="s">
+      <c r="I6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="7" t="s">
+      <c r="K6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="M6" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="M6" s="8"/>
-      <c r="Q6" s="8"/>
+      <c r="N6" s="7"/>
+      <c r="R6" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -782,9 +805,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -966,26 +992,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE1791-BEC8-419B-A7D8-F7EAC9E3F094}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -1009,9 +1024,17 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7613A94-47D1-485D-A76D-D3A6CFAB63B4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4EFE1791-BEC8-419B-A7D8-F7EAC9E3F094}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="aa5be1c8-7296-4b7a-853c-c6802fcefdea"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>